<commit_message>
Interest form UI completed
</commit_message>
<xml_diff>
--- a/public/csk_initial_data.xlsx
+++ b/public/csk_initial_data.xlsx
@@ -5,26 +5,27 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksh\OneDrive - Concordia University - Canada\Documents\github\csk-share-replica-nextjs\csk-share-replica-nextjs\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F3D14-C3E8-4343-80A6-AA4FDED93B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F527DE60-B742-4476-B139-FE970976FC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Fundamentals" sheetId="1" r:id="rId1"/>
-    <sheet name="Financials" sheetId="2" r:id="rId2"/>
-    <sheet name="Financial Ratios" sheetId="3" r:id="rId3"/>
-    <sheet name="Shareholding Pattern" sheetId="4" r:id="rId4"/>
-    <sheet name="Promoters or Management" sheetId="5" r:id="rId5"/>
+    <sheet name="Share_Price" sheetId="6" r:id="rId1"/>
+    <sheet name="Fundamentals" sheetId="1" r:id="rId2"/>
+    <sheet name="Financials" sheetId="2" r:id="rId3"/>
+    <sheet name="Financial_Ratios" sheetId="3" r:id="rId4"/>
+    <sheet name="Shareholding_Pattern" sheetId="4" r:id="rId5"/>
+    <sheet name="Promoters_or_Management" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="94">
   <si>
     <t>Parameter</t>
   </si>
@@ -291,6 +292,21 @@
   </si>
   <si>
     <t>30 yrs</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>Diff_Percentage</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>4M</t>
   </si>
 </sst>
 </file>
@@ -349,11 +365,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,11 +674,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F3127E-5015-421E-9501-3B66F15A7DA8}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>188</v>
+      </c>
+      <c r="B2">
+        <v>-30</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-0.13800000000000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,345 +886,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2">
-        <v>24783</v>
-      </c>
-      <c r="C2">
-        <v>34105</v>
-      </c>
-      <c r="D2">
-        <v>27315</v>
-      </c>
-      <c r="E2">
-        <v>69545</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3">
-        <v>17941</v>
-      </c>
-      <c r="C3">
-        <v>281559</v>
-      </c>
-      <c r="D3">
-        <v>20161</v>
-      </c>
-      <c r="E3">
-        <v>41841</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <v>26.61</v>
-      </c>
-      <c r="C4">
-        <v>17.43</v>
-      </c>
-      <c r="D4">
-        <v>26.19</v>
-      </c>
-      <c r="E4">
-        <v>39.840000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6">
-        <v>247</v>
-      </c>
-      <c r="C6">
-        <v>318</v>
-      </c>
-      <c r="D6">
-        <v>368</v>
-      </c>
-      <c r="E6">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7">
-        <v>400</v>
-      </c>
-      <c r="C7">
-        <v>1495</v>
-      </c>
-      <c r="D7">
-        <v>284</v>
-      </c>
-      <c r="E7">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8">
-        <v>6195</v>
-      </c>
-      <c r="C8">
-        <v>4133</v>
-      </c>
-      <c r="D8">
-        <v>6502</v>
-      </c>
-      <c r="E8">
-        <v>26364</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9">
-        <v>25</v>
-      </c>
-      <c r="C9">
-        <v>12012</v>
-      </c>
-      <c r="D9">
-        <v>23.8</v>
-      </c>
-      <c r="E9">
-        <v>37.909999999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10">
-        <v>586</v>
-      </c>
-      <c r="C10">
-        <v>8809</v>
-      </c>
-      <c r="D10">
-        <v>1919</v>
-      </c>
-      <c r="E10">
-        <v>2783</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11">
-        <v>526</v>
-      </c>
-      <c r="C11">
-        <v>567</v>
-      </c>
-      <c r="D11">
-        <v>1005</v>
-      </c>
-      <c r="E11">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12">
-        <v>333</v>
-      </c>
-      <c r="C12">
-        <v>240</v>
-      </c>
-      <c r="D12">
-        <v>363</v>
-      </c>
-      <c r="E12">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13">
-        <v>5862</v>
-      </c>
-      <c r="C13">
-        <v>3893</v>
-      </c>
-      <c r="D13">
-        <v>6139</v>
-      </c>
-      <c r="E13">
-        <v>25890</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14">
-        <v>23.65</v>
-      </c>
-      <c r="C14">
-        <v>11.41</v>
-      </c>
-      <c r="D14">
-        <v>22.47</v>
-      </c>
-      <c r="E14">
-        <v>37.229999999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15">
-        <v>5919</v>
-      </c>
-      <c r="C15">
-        <v>4133</v>
-      </c>
-      <c r="D15">
-        <v>7053</v>
-      </c>
-      <c r="E15">
-        <v>27916</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16">
-        <v>1893</v>
-      </c>
-      <c r="C16">
-        <v>920</v>
-      </c>
-      <c r="D16">
-        <v>1835</v>
-      </c>
-      <c r="E16">
-        <v>7766</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17">
-        <v>4026</v>
-      </c>
-      <c r="C17">
-        <v>3213</v>
-      </c>
-      <c r="D17">
-        <v>5218</v>
-      </c>
-      <c r="E17">
-        <v>20150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18">
-        <v>16.25</v>
-      </c>
-      <c r="C18">
-        <v>9.42</v>
-      </c>
-      <c r="D18">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="E18">
-        <v>28.97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19">
-        <v>1.31</v>
-      </c>
-      <c r="C19">
-        <v>1.04</v>
-      </c>
-      <c r="D19">
-        <v>1.69</v>
-      </c>
-      <c r="E19">
-        <v>5.32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1172,7 +896,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>
@@ -1189,52 +913,307 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B2">
-        <v>25</v>
+        <v>24783</v>
       </c>
       <c r="C2">
-        <v>12.12</v>
+        <v>34105</v>
       </c>
       <c r="D2">
-        <v>23.8</v>
+        <v>27315</v>
       </c>
       <c r="E2">
-        <v>37.909999999999997</v>
+        <v>69545</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B3">
-        <v>16.25</v>
+        <v>17941</v>
       </c>
       <c r="C3">
-        <v>9.42</v>
+        <v>281559</v>
       </c>
       <c r="D3">
-        <v>19.100000000000001</v>
+        <v>20161</v>
       </c>
       <c r="E3">
-        <v>28.7</v>
+        <v>41841</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B4">
+        <v>26.61</v>
+      </c>
+      <c r="C4">
+        <v>17.43</v>
+      </c>
+      <c r="D4">
+        <v>26.19</v>
+      </c>
+      <c r="E4">
+        <v>39.840000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <v>247</v>
+      </c>
+      <c r="C6">
+        <v>318</v>
+      </c>
+      <c r="D6">
+        <v>368</v>
+      </c>
+      <c r="E6">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>400</v>
+      </c>
+      <c r="C7">
+        <v>1495</v>
+      </c>
+      <c r="D7">
+        <v>284</v>
+      </c>
+      <c r="E7">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>6195</v>
+      </c>
+      <c r="C8">
+        <v>4133</v>
+      </c>
+      <c r="D8">
+        <v>6502</v>
+      </c>
+      <c r="E8">
+        <v>26364</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>12012</v>
+      </c>
+      <c r="D9">
+        <v>23.8</v>
+      </c>
+      <c r="E9">
+        <v>37.909999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10">
+        <v>586</v>
+      </c>
+      <c r="C10">
+        <v>8809</v>
+      </c>
+      <c r="D10">
+        <v>1919</v>
+      </c>
+      <c r="E10">
+        <v>2783</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>526</v>
+      </c>
+      <c r="C11">
+        <v>567</v>
+      </c>
+      <c r="D11">
+        <v>1005</v>
+      </c>
+      <c r="E11">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>333</v>
+      </c>
+      <c r="C12">
+        <v>240</v>
+      </c>
+      <c r="D12">
+        <v>363</v>
+      </c>
+      <c r="E12">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13">
+        <v>5862</v>
+      </c>
+      <c r="C13">
+        <v>3893</v>
+      </c>
+      <c r="D13">
+        <v>6139</v>
+      </c>
+      <c r="E13">
+        <v>25890</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14">
+        <v>23.65</v>
+      </c>
+      <c r="C14">
+        <v>11.41</v>
+      </c>
+      <c r="D14">
+        <v>22.47</v>
+      </c>
+      <c r="E14">
+        <v>37.229999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15">
+        <v>5919</v>
+      </c>
+      <c r="C15">
+        <v>4133</v>
+      </c>
+      <c r="D15">
+        <v>7053</v>
+      </c>
+      <c r="E15">
+        <v>27916</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16">
+        <v>1893</v>
+      </c>
+      <c r="C16">
+        <v>920</v>
+      </c>
+      <c r="D16">
+        <v>1835</v>
+      </c>
+      <c r="E16">
+        <v>7766</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17">
+        <v>4026</v>
+      </c>
+      <c r="C17">
+        <v>3213</v>
+      </c>
+      <c r="D17">
+        <v>5218</v>
+      </c>
+      <c r="E17">
+        <v>20150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <v>16.25</v>
+      </c>
+      <c r="C18">
+        <v>9.42</v>
+      </c>
+      <c r="D18">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E18">
+        <v>28.97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19">
         <v>1.31</v>
       </c>
-      <c r="C4">
+      <c r="C19">
         <v>1.04</v>
       </c>
-      <c r="D4">
+      <c r="D19">
         <v>1.69</v>
       </c>
-      <c r="E4">
+      <c r="E19">
         <v>5.32</v>
       </c>
     </row>
@@ -1244,6 +1223,89 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>12.12</v>
+      </c>
+      <c r="D2">
+        <v>23.8</v>
+      </c>
+      <c r="E2">
+        <v>37.909999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>16.25</v>
+      </c>
+      <c r="C3">
+        <v>9.42</v>
+      </c>
+      <c r="D3">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E3">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>1.31</v>
+      </c>
+      <c r="C4">
+        <v>1.04</v>
+      </c>
+      <c r="D4">
+        <v>1.69</v>
+      </c>
+      <c r="E4">
+        <v>5.32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -1363,7 +1425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>